<commit_message>
listados completos del 29 de julio de 2024
</commit_message>
<xml_diff>
--- a/Julio/27 julio/papaloapan/PLANTILLA LISTA DE ASPIRANTES_SIMULACRO 23-07-24 (1).xlsx
+++ b/Julio/27 julio/papaloapan/PLANTILLA LISTA DE ASPIRANTES_SIMULACRO 23-07-24 (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proyecto01TICs\Documents\Evaluatec2024\Julio\27 julio\papaloapan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxoC\OneDrive\Documents\EVALUATEC2024\Julio\27 julio\papaloapan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171E54AD-3381-44C3-970E-72EF8DA2C496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D5E572-D0B0-4AA4-B748-429DAEA66A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVALUATEC" sheetId="1" r:id="rId1"/>
@@ -1099,7 +1099,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1146,9 +1146,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1156,13 +1153,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="h:mm\ AM/PM"/>
     </dxf>
@@ -1208,22 +1226,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:M104" totalsRowShown="0">
   <autoFilter ref="A1:M104" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M104">
-    <sortCondition ref="F1:F104"/>
+    <sortCondition ref="A1:A104"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FICHA"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NOMBRE ASPIRANTE"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CURP"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CORREO ELECTRONICO"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="CLAVE CARRERA" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="CLAVE CARRERA" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="CARRERA"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="VERSION" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FECHA SIMULACRO" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="HORA DE SIMULACRO" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="AULA" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="VERSION" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="FECHA SIMULACRO" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="HORA DE SIMULACRO" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="FECHA APLICACIÓN OFICIAL" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="HORA APLICACIÓN OFICIAL" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="¿ASPIRANTE EN PLANTEL?" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="AULA" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1531,7 +1549,9 @@
   </sheetPr>
   <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D34" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1593,20 +1613,20 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>79</v>
+        <v>227</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>80</v>
+        <v>229</v>
       </c>
       <c r="E2" s="14"/>
-      <c r="F2" s="7" t="s">
-        <v>81</v>
+      <c r="F2" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>13</v>
@@ -1630,20 +1650,20 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
-        <v>180</v>
+        <v>3</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>102</v>
+        <v>73</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>74</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="7" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>13</v>
@@ -1667,20 +1687,20 @@
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
-        <v>203</v>
+        <v>8</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>205</v>
+        <v>49</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>206</v>
+        <v>50</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>207</v>
+        <v>51</v>
       </c>
       <c r="E4" s="14"/>
-      <c r="F4" s="17" t="s">
-        <v>81</v>
+      <c r="F4" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>13</v>
@@ -1704,20 +1724,20 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>224</v>
+        <v>52</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>225</v>
+        <v>53</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>226</v>
+        <v>54</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="17" t="s">
-        <v>81</v>
+      <c r="F5" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>13</v>
@@ -1738,27 +1758,27 @@
         <v>14</v>
       </c>
       <c r="M5" s="3"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
-        <v>210</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>230</v>
+        <v>11</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>231</v>
+        <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="11">
@@ -1776,26 +1796,26 @@
       <c r="L6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="3"/>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
-        <v>221</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>263</v>
+        <v>12</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>264</v>
+        <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="11">
@@ -1813,24 +1833,24 @@
       <c r="L7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="3"/>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>235</v>
+        <v>14</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>305</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>306</v>
+        <v>58</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="16" t="s">
-        <v>81</v>
+        <v>59</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>13</v>
@@ -1854,53 +1874,53 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <v>11</v>
-      </c>
-      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="11">
+        <v>45496</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="13">
+        <v>45500</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>21</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="11">
-        <v>45496</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="13">
-        <v>45500</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="6"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
-        <v>88</v>
-      </c>
       <c r="B10" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>27</v>
+        <v>140</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>142</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="7" t="s">
@@ -1927,17 +1947,17 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
-        <v>95</v>
+      <c r="A11" s="7">
+        <v>29</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>30</v>
+        <v>107</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="7" t="s">
@@ -1964,17 +1984,17 @@
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
-        <v>60</v>
+      <c r="A12" s="7">
+        <v>38</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>33</v>
+        <v>143</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="7" t="s">
@@ -2001,21 +2021,21 @@
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
-        <v>105</v>
+      <c r="A13" s="7">
+        <v>40</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>36</v>
+        <v>110</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>13</v>
@@ -2038,17 +2058,17 @@
       <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
-        <v>99</v>
+      <c r="A14" s="7">
+        <v>48</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>41</v>
+        <v>105</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>106</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="7" t="s">
@@ -2076,16 +2096,16 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>78</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="7" t="s">
@@ -2113,16 +2133,16 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
-        <v>172</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>46</v>
+        <v>54</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>48</v>
+        <v>131</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>133</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="7" t="s">
@@ -2150,20 +2170,20 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>54</v>
+        <v>115</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>114</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>13</v>
@@ -2186,17 +2206,17 @@
       <c r="M17" s="3"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>61</v>
+      <c r="A18" s="16">
+        <v>60</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>57</v>
+        <v>31</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>33</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="7" t="s">
@@ -2224,16 +2244,16 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>57</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="7" t="s">
@@ -2261,16 +2281,16 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>62</v>
+        <v>134</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>136</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="7" t="s">
@@ -2298,20 +2318,20 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
-        <v>173</v>
+        <v>80</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>66</v>
+        <v>98</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>13</v>
@@ -2335,16 +2355,16 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>174</v>
+        <v>83</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>68</v>
+        <v>61</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="7" t="s">
@@ -2372,16 +2392,16 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>75</v>
+        <v>116</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>118</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="7" t="s">
@@ -2408,17 +2428,17 @@
       <c r="M23" s="3"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
-        <v>52</v>
+      <c r="A24" s="16">
+        <v>88</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>78</v>
+        <v>25</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>27</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="7" t="s">
@@ -2446,16 +2466,16 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>85</v>
+        <v>137</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>139</v>
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="7" t="s">
@@ -2482,17 +2502,17 @@
       <c r="M25" s="3"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
-        <v>126</v>
+      <c r="A26" s="16">
+        <v>95</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>88</v>
+        <v>28</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>30</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="7" t="s">
@@ -2520,16 +2540,16 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
-        <v>175</v>
+        <v>98</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>90</v>
+        <v>43</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>45</v>
       </c>
       <c r="E27" s="14"/>
       <c r="F27" s="7" t="s">
@@ -2556,17 +2576,17 @@
       <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
-        <v>176</v>
+      <c r="A28" s="16">
+        <v>99</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>92</v>
+        <v>42</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="7" t="s">
@@ -2594,20 +2614,20 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="23" t="s">
-        <v>96</v>
+        <v>70</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>71</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>13</v>
@@ -2630,17 +2650,17 @@
       <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
-        <v>48</v>
+      <c r="A30" s="16">
+        <v>105</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>106</v>
+        <v>34</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>36</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="7" t="s">
@@ -2668,20 +2688,20 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>108</v>
+        <v>82</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>79</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="7" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>13</v>
@@ -2705,16 +2725,16 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>117</v>
+        <v>83</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>84</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="7" t="s">
@@ -2742,16 +2762,16 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
-        <v>180</v>
+        <v>125</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C33" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" s="24" t="s">
-        <v>132</v>
+        <v>146</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>148</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="7" t="s">
@@ -2779,16 +2799,16 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
-        <v>181</v>
+        <v>126</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>123</v>
+        <v>86</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>88</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="7" t="s">
@@ -2815,21 +2835,21 @@
       <c r="M34" s="3"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
-        <v>182</v>
+      <c r="A35" s="16">
+        <v>171</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>126</v>
+        <v>37</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>13</v>
@@ -2853,16 +2873,16 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
-        <v>183</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>127</v>
+        <v>172</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>46</v>
       </c>
       <c r="C36" t="s">
-        <v>128</v>
-      </c>
-      <c r="D36" s="24" t="s">
-        <v>129</v>
+        <v>47</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>48</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="7" t="s">
@@ -2890,16 +2910,16 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C37" t="s">
-        <v>131</v>
-      </c>
-      <c r="D37" s="24" t="s">
-        <v>133</v>
+        <v>65</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="7" t="s">
@@ -2927,16 +2947,16 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
+        <v>174</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>136</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="7" t="s">
@@ -2964,16 +2984,16 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
-        <v>93</v>
+        <v>175</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>138</v>
+        <v>91</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>89</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
       <c r="E39" s="14"/>
       <c r="F39" s="7" t="s">
@@ -3001,16 +3021,16 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <v>21</v>
+        <v>176</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="C40" s="23" t="s">
-        <v>141</v>
+        <v>94</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>92</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>142</v>
+        <v>93</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="7" t="s">
@@ -3038,20 +3058,20 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
-        <v>38</v>
+        <v>180</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>144</v>
+        <v>101</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="E41" s="14"/>
       <c r="F41" s="7" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>13</v>
@@ -3075,16 +3095,16 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
-        <v>125</v>
+        <v>1800</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>148</v>
+        <v>119</v>
+      </c>
+      <c r="C42" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>132</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="7" t="s">
@@ -3112,16 +3132,16 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="C43" t="s">
-        <v>151</v>
-      </c>
-      <c r="D43" s="24" t="s">
-        <v>149</v>
+        <v>122</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>123</v>
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="7" t="s">
@@ -3149,16 +3169,16 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C44" t="s">
-        <v>153</v>
-      </c>
-      <c r="D44" s="24" t="s">
-        <v>154</v>
+        <v>125</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>126</v>
       </c>
       <c r="E44" s="14"/>
       <c r="F44" s="7" t="s">
@@ -3186,16 +3206,16 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="E45" s="14"/>
       <c r="F45" s="7" t="s">
@@ -3223,16 +3243,16 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="7" t="s">
@@ -3260,16 +3280,16 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="7" t="s">
@@ -3297,16 +3317,16 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="7" t="s">
@@ -3334,16 +3354,16 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="7" t="s">
@@ -3371,16 +3391,16 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="7" t="s">
@@ -3408,20 +3428,20 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>211</v>
+        <v>164</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="E51" s="14"/>
-      <c r="F51" s="7" t="s">
-        <v>24</v>
+      <c r="F51" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="G51" s="17" t="s">
         <v>13</v>
@@ -3445,16 +3465,16 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="E52" s="14"/>
       <c r="F52" s="7" t="s">
@@ -3482,16 +3502,16 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="E53" s="14"/>
       <c r="F53" s="7" t="s">
@@ -3519,16 +3539,16 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="7" t="s">
@@ -3556,16 +3576,16 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="E55" s="14"/>
       <c r="F55" s="7" t="s">
@@ -3593,16 +3613,16 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="E56" s="14"/>
       <c r="F56" s="7" t="s">
@@ -3630,16 +3650,16 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="E57" s="14"/>
       <c r="F57" s="7" t="s">
@@ -3667,16 +3687,16 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="E58" s="14"/>
       <c r="F58" s="7" t="s">
@@ -3704,16 +3724,16 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="E59" s="14"/>
       <c r="F59" s="7" t="s">
@@ -3741,16 +3761,16 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="E60" s="14"/>
       <c r="F60" s="7" t="s">
@@ -3778,20 +3798,20 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>234</v>
+        <v>193</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="E61" s="14"/>
-      <c r="F61" s="7" t="s">
-        <v>24</v>
+      <c r="F61" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="G61" s="17" t="s">
         <v>13</v>
@@ -3815,20 +3835,20 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>237</v>
+        <v>197</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>238</v>
+        <v>198</v>
       </c>
       <c r="E62" s="14"/>
-      <c r="F62" s="7" t="s">
-        <v>24</v>
+      <c r="F62" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="G62" s="17" t="s">
         <v>13</v>
@@ -3852,16 +3872,16 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>239</v>
+        <v>199</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
       <c r="E63" s="14"/>
       <c r="F63" s="7" t="s">
@@ -3889,20 +3909,20 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>242</v>
+        <v>202</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>243</v>
+        <v>203</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>244</v>
+        <v>204</v>
       </c>
       <c r="E64" s="14"/>
-      <c r="F64" s="7" t="s">
-        <v>24</v>
+      <c r="F64" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="G64" s="17" t="s">
         <v>13</v>
@@ -3926,20 +3946,20 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>247</v>
+        <v>206</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>246</v>
+        <v>207</v>
       </c>
       <c r="E65" s="14"/>
-      <c r="F65" s="7" t="s">
-        <v>24</v>
+      <c r="F65" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="G65" s="17" t="s">
         <v>13</v>
@@ -3963,16 +3983,16 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>248</v>
+        <v>208</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>249</v>
+        <v>209</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>250</v>
+        <v>210</v>
       </c>
       <c r="E66" s="14"/>
       <c r="F66" s="7" t="s">
@@ -4000,16 +4020,16 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>251</v>
+        <v>212</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>252</v>
+        <v>213</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>253</v>
+        <v>214</v>
       </c>
       <c r="E67" s="14"/>
       <c r="F67" s="7" t="s">
@@ -4037,16 +4057,16 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>254</v>
+        <v>215</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>255</v>
+        <v>216</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>256</v>
+        <v>217</v>
       </c>
       <c r="E68" s="14"/>
       <c r="F68" s="7" t="s">
@@ -4074,16 +4094,16 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
+        <v>207</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C69" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="B69" s="16" t="s">
-        <v>257</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>258</v>
-      </c>
       <c r="D69" s="8" t="s">
-        <v>259</v>
+        <v>220</v>
       </c>
       <c r="E69" s="14"/>
       <c r="F69" s="7" t="s">
@@ -4111,20 +4131,20 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>260</v>
+        <v>221</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>261</v>
+        <v>222</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>262</v>
+        <v>223</v>
       </c>
       <c r="E70" s="14"/>
-      <c r="F70" s="7" t="s">
-        <v>24</v>
+      <c r="F70" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="G70" s="17" t="s">
         <v>13</v>
@@ -4148,20 +4168,20 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>266</v>
+        <v>224</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>267</v>
+        <v>225</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>268</v>
+        <v>226</v>
       </c>
       <c r="E71" s="14"/>
-      <c r="F71" s="7" t="s">
-        <v>24</v>
+      <c r="F71" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="G71" s="17" t="s">
         <v>13</v>
@@ -4185,20 +4205,20 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>269</v>
+        <v>230</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>270</v>
+        <v>231</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>271</v>
+        <v>232</v>
       </c>
       <c r="E72" s="14"/>
-      <c r="F72" s="7" t="s">
-        <v>24</v>
+      <c r="F72" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="G72" s="17" t="s">
         <v>13</v>
@@ -4222,16 +4242,16 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>272</v>
+        <v>233</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>274</v>
+        <v>235</v>
       </c>
       <c r="E73" s="14"/>
       <c r="F73" s="7" t="s">
@@ -4259,16 +4279,16 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>275</v>
+        <v>236</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>277</v>
+        <v>238</v>
       </c>
       <c r="E74" s="14"/>
       <c r="F74" s="7" t="s">
@@ -4296,16 +4316,16 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>278</v>
+        <v>239</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>279</v>
+        <v>240</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>280</v>
+        <v>241</v>
       </c>
       <c r="E75" s="14"/>
       <c r="F75" s="7" t="s">
@@ -4333,16 +4353,16 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>281</v>
+        <v>242</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>282</v>
+        <v>243</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>283</v>
+        <v>244</v>
       </c>
       <c r="E76" s="14"/>
       <c r="F76" s="7" t="s">
@@ -4370,18 +4390,18 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>290</v>
+        <v>245</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>291</v>
+        <v>247</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="E77" s="18"/>
+        <v>246</v>
+      </c>
+      <c r="E77" s="14"/>
       <c r="F77" s="7" t="s">
         <v>24</v>
       </c>
@@ -4407,18 +4427,18 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>293</v>
+        <v>248</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>294</v>
+        <v>249</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="E78" s="18"/>
+        <v>250</v>
+      </c>
+      <c r="E78" s="14"/>
       <c r="F78" s="7" t="s">
         <v>24</v>
       </c>
@@ -4444,18 +4464,18 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>296</v>
+        <v>251</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>297</v>
+        <v>252</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="E79" s="18"/>
+        <v>253</v>
+      </c>
+      <c r="E79" s="14"/>
       <c r="F79" s="7" t="s">
         <v>24</v>
       </c>
@@ -4481,18 +4501,18 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>299</v>
+        <v>254</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>300</v>
+        <v>255</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="E80" s="18"/>
+        <v>256</v>
+      </c>
+      <c r="E80" s="14"/>
       <c r="F80" s="7" t="s">
         <v>24</v>
       </c>
@@ -4518,18 +4538,18 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="E81" s="18"/>
+        <v>259</v>
+      </c>
+      <c r="E81" s="14"/>
       <c r="F81" s="7" t="s">
         <v>24</v>
       </c>
@@ -4555,18 +4575,18 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>308</v>
+        <v>260</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>309</v>
+        <v>261</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="E82" s="18"/>
+        <v>262</v>
+      </c>
+      <c r="E82" s="14"/>
       <c r="F82" s="7" t="s">
         <v>24</v>
       </c>
@@ -4592,20 +4612,20 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>311</v>
+        <v>263</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>312</v>
+        <v>264</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="E83" s="18"/>
-      <c r="F83" s="7" t="s">
-        <v>24</v>
+        <v>265</v>
+      </c>
+      <c r="E83" s="14"/>
+      <c r="F83" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="G83" s="17" t="s">
         <v>13</v>
@@ -4629,18 +4649,18 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>314</v>
+        <v>266</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>315</v>
+        <v>267</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="E84" s="18"/>
+        <v>268</v>
+      </c>
+      <c r="E84" s="14"/>
       <c r="F84" s="7" t="s">
         <v>24</v>
       </c>
@@ -4666,18 +4686,18 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>317</v>
+        <v>269</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>318</v>
+        <v>270</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="E85" s="18"/>
+        <v>271</v>
+      </c>
+      <c r="E85" s="14"/>
       <c r="F85" s="7" t="s">
         <v>24</v>
       </c>
@@ -4703,18 +4723,18 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>320</v>
+        <v>272</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>321</v>
+        <v>273</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="E86" s="18"/>
+        <v>274</v>
+      </c>
+      <c r="E86" s="14"/>
       <c r="F86" s="7" t="s">
         <v>24</v>
       </c>
@@ -4740,18 +4760,18 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>323</v>
+        <v>275</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>324</v>
+        <v>276</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="E87" s="18"/>
+        <v>277</v>
+      </c>
+      <c r="E87" s="14"/>
       <c r="F87" s="7" t="s">
         <v>24</v>
       </c>
@@ -4777,18 +4797,18 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>326</v>
+        <v>278</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>327</v>
+        <v>279</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="E88" s="18"/>
+        <v>280</v>
+      </c>
+      <c r="E88" s="14"/>
       <c r="F88" s="7" t="s">
         <v>24</v>
       </c>
@@ -4814,16 +4834,16 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
-        <v>191</v>
+        <v>227</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>170</v>
+        <v>281</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>171</v>
+        <v>282</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>172</v>
+        <v>283</v>
       </c>
       <c r="E89" s="14"/>
       <c r="F89" s="7" t="s">
@@ -4851,22 +4871,22 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
-        <v>12</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>17</v>
+        <v>228</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>284</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>18</v>
+        <v>285</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E90" s="9"/>
-      <c r="F90" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="E90" s="14"/>
+      <c r="F90" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G90" s="10" t="s">
+      <c r="G90" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H90" s="11">
@@ -4884,23 +4904,23 @@
       <c r="L90" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="M90" s="6"/>
+      <c r="M90" s="3"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" s="16">
-        <v>171</v>
+      <c r="A91" s="7">
+        <v>229</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C91" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D91" s="19" t="s">
-        <v>39</v>
+        <v>287</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>289</v>
       </c>
       <c r="E91" s="14"/>
-      <c r="F91" s="7" t="s">
+      <c r="F91" s="17" t="s">
         <v>20</v>
       </c>
       <c r="G91" s="17" t="s">
@@ -4925,20 +4945,20 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
-        <v>8</v>
+        <v>230</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>49</v>
+        <v>290</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>50</v>
+        <v>291</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E92" s="14"/>
+        <v>292</v>
+      </c>
+      <c r="E92" s="18"/>
       <c r="F92" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G92" s="17" t="s">
         <v>13</v>
@@ -4962,20 +4982,20 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
-        <v>103</v>
+        <v>231</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C93" s="23" t="s">
-        <v>71</v>
+        <v>293</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>294</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E93" s="14"/>
+        <v>295</v>
+      </c>
+      <c r="E93" s="18"/>
       <c r="F93" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G93" s="17" t="s">
         <v>13</v>
@@ -4999,20 +5019,20 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
-        <v>80</v>
+        <v>232</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>98</v>
+        <v>296</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>99</v>
+        <v>297</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E94" s="14"/>
+        <v>298</v>
+      </c>
+      <c r="E94" s="18"/>
       <c r="F94" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G94" s="17" t="s">
         <v>13</v>
@@ -5036,20 +5056,20 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
-        <v>40</v>
+        <v>233</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>110</v>
+        <v>299</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>111</v>
+        <v>300</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E95" s="14"/>
+        <v>301</v>
+      </c>
+      <c r="E95" s="18"/>
       <c r="F95" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G95" s="17" t="s">
         <v>13</v>
@@ -5073,20 +5093,20 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
-        <v>56</v>
+        <v>234</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="C96" s="23" t="s">
-        <v>113</v>
+        <v>302</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>303</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E96" s="14"/>
+        <v>304</v>
+      </c>
+      <c r="E96" s="18"/>
       <c r="F96" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G96" s="17" t="s">
         <v>13</v>
@@ -5110,20 +5130,20 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>164</v>
+        <v>305</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>165</v>
+        <v>306</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="E97" s="14"/>
-      <c r="F97" s="17" t="s">
-        <v>20</v>
+        <v>307</v>
+      </c>
+      <c r="E97" s="18"/>
+      <c r="F97" s="16" t="s">
+        <v>81</v>
       </c>
       <c r="G97" s="17" t="s">
         <v>13</v>
@@ -5147,20 +5167,20 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
-        <v>199</v>
+        <v>236</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>194</v>
+        <v>308</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>193</v>
+        <v>309</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="E98" s="14"/>
-      <c r="F98" s="17" t="s">
-        <v>20</v>
+        <v>310</v>
+      </c>
+      <c r="E98" s="18"/>
+      <c r="F98" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G98" s="17" t="s">
         <v>13</v>
@@ -5184,20 +5204,20 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
-        <v>200</v>
+        <v>237</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>196</v>
+        <v>311</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>197</v>
+        <v>312</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="E99" s="14"/>
-      <c r="F99" s="17" t="s">
-        <v>20</v>
+        <v>313</v>
+      </c>
+      <c r="E99" s="18"/>
+      <c r="F99" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G99" s="17" t="s">
         <v>13</v>
@@ -5221,20 +5241,20 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
-        <v>202</v>
+        <v>238</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>202</v>
+        <v>314</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>203</v>
+        <v>315</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="E100" s="14"/>
-      <c r="F100" s="17" t="s">
-        <v>20</v>
+        <v>316</v>
+      </c>
+      <c r="E100" s="18"/>
+      <c r="F100" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G100" s="17" t="s">
         <v>13</v>
@@ -5258,20 +5278,20 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
-        <v>208</v>
+        <v>239</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>221</v>
+        <v>317</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>222</v>
+        <v>318</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="E101" s="14"/>
-      <c r="F101" s="17" t="s">
-        <v>20</v>
+        <v>319</v>
+      </c>
+      <c r="E101" s="18"/>
+      <c r="F101" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G101" s="17" t="s">
         <v>13</v>
@@ -5295,20 +5315,20 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
-        <v>1</v>
+        <v>240</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>227</v>
+        <v>320</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>228</v>
+        <v>321</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="E102" s="14"/>
-      <c r="F102" s="17" t="s">
-        <v>20</v>
+        <v>322</v>
+      </c>
+      <c r="E102" s="18"/>
+      <c r="F102" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G102" s="17" t="s">
         <v>13</v>
@@ -5332,20 +5352,20 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>284</v>
+        <v>323</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="E103" s="14"/>
-      <c r="F103" s="17" t="s">
-        <v>20</v>
+        <v>325</v>
+      </c>
+      <c r="E103" s="18"/>
+      <c r="F103" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G103" s="17" t="s">
         <v>13</v>
@@ -5369,20 +5389,20 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>287</v>
+        <v>326</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>288</v>
+        <v>327</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="E104" s="14"/>
-      <c r="F104" s="17" t="s">
-        <v>20</v>
+        <v>328</v>
+      </c>
+      <c r="E104" s="18"/>
+      <c r="F104" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="G104" s="17" t="s">
         <v>13</v>
@@ -5408,110 +5428,113 @@
   <mergeCells count="1">
     <mergeCell ref="N5:O5"/>
   </mergeCells>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D90" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D91" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D14" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D15" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D92" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="D17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D94" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D3" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D30" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D31" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D95" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D36" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D33" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D37" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D38" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="D39" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D41" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D40" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="D35" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D34" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="D32" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D96" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D29" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="D27" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="D28" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D26" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="D25" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="D2" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="D24" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="D23" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="D93" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="D22" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="D21" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="D20" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="D19" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="D18" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="D44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="D45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="D46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="D47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="D97" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="D48" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="D89" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="D49" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="D50" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="D51" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="D52" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="D53" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D54" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="D43" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="D42" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="D55" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="D98" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="D99" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="D56" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="D100" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="D4" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="D57" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="D58" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="D59" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="D60" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="D101" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D5" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="D102" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="D6" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="D61" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="D62" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="D63" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="D64" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="D65" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="D66" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="D67" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="D68" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="D69" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="D70" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="D7" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="D71" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="D72" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="D73" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="D74" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="D75" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="D76" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="D103" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="D104" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="D77" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="D78" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D79" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="D80" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="D81" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="D8" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="D82" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="D83" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="D84" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="D85" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="D86" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="D87" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="D88" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D26" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D18" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D30" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D35" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D28" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D27" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D5" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D41" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D14" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D11" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D45" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D42" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D16" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D20" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D12" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D10" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D44" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D43" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D23" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D17" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D9" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D39" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="D40" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D32" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="D31" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="D15" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="D3" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="D29" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D38" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="D37" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="D22" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="D8" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D19" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="D47" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="D48" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="D49" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="D50" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D51" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="D52" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="D53" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="D54" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="D55" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="D56" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="D57" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="D58" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="D59" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="D46" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="D33" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="D60" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="D61" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="D62" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="D63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="D64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="D65" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="D66" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="D67" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="D68" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="D69" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="D70" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D71" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="D2" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="D72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="D73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="D74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="D75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="D76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="D77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="D78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="D79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="D80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="D81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="D82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="D83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="D84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="D85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="D86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="D87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="D88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="D89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="D90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="D91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="D92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="D93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="D94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="D95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="D96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="D97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="D98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="D99" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="D100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="D101" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="D102" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="D103" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="D104" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape"/>

</xml_diff>